<commit_message>
noted on candidate region for tile buffer
</commit_message>
<xml_diff>
--- a/docs/development/wram-utilizations.xlsx
+++ b/docs/development/wram-utilizations.xlsx
@@ -449,12 +449,18 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -471,11 +477,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -764,7 +773,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -849,7 +858,7 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="H2" s="1" t="str">
+      <c r="H2" s="2" t="str">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
@@ -915,7 +924,7 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>0</v>
       </c>
       <c r="I3" s="1">
@@ -965,7 +974,7 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="1">
@@ -1018,7 +1027,7 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="1">
@@ -1071,7 +1080,7 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="1">
@@ -1124,7 +1133,7 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="1">
@@ -1174,7 +1183,7 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="1">
@@ -1227,7 +1236,7 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>0</v>
       </c>
       <c r="I9" s="1">
@@ -1277,7 +1286,7 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>0</v>
       </c>
       <c r="I10" s="1">
@@ -1327,7 +1336,7 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="1">
@@ -1380,7 +1389,7 @@
       <c r="G12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>0</v>
       </c>
       <c r="I12" s="1">
@@ -1433,7 +1442,7 @@
       <c r="G13" s="1">
         <v>1</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>1</v>
       </c>
       <c r="I13" s="1">
@@ -1475,6 +1484,9 @@
       <c r="U13" s="1" t="s">
         <v>63</v>
       </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
@@ -1499,7 +1511,7 @@
       <c r="G15" s="1">
         <v>2</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>0</v>
       </c>
       <c r="I15" s="1">
@@ -1553,7 +1565,7 @@
       <c r="G16" s="1">
         <v>2</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <v>0</v>
       </c>
       <c r="I16" s="1">
@@ -1610,7 +1622,7 @@
       <c r="G17" s="1">
         <v>2</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="2">
         <v>0</v>
       </c>
       <c r="I17" s="1">
@@ -1667,7 +1679,7 @@
       <c r="G18" s="1">
         <v>2</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <v>0</v>
       </c>
       <c r="I18" s="1">
@@ -1721,7 +1733,7 @@
       <c r="G19" s="1">
         <v>2</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="1">

</xml_diff>